<commit_message>
Interpolacja akima i wybór sprawny, problemy z ilością próbek w liniowej
</commit_message>
<xml_diff>
--- a/src/excel_datas/data3.xlsx
+++ b/src/excel_datas/data3.xlsx
@@ -20,30 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">X</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">125.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">126.6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">128.6</t>
   </si>
 </sst>
 </file>
@@ -151,10 +133,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -176,48 +158,48 @@
       <c r="A3" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
+      <c r="B3" s="2" t="n">
+        <v>100.5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
+      <c r="B4" s="2" t="n">
+        <v>120.3</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
+      <c r="B5" s="2" t="n">
+        <v>125.7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
+      <c r="B6" s="2" t="n">
+        <v>126.6</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
+      <c r="B7" s="2" t="n">
+        <v>127.5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
+      <c r="B8" s="2" t="n">
+        <v>128.6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>